<commit_message>
Codigo de carga terminado
</commit_message>
<xml_diff>
--- a/matrices.xlsx
+++ b/matrices.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22254ca56b479b7e/Coding/MuscleApp/gymAPP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nical\OneDrive\Coding\MuscleApp\gymAPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="11_F25DC773A252ABDACC104897891B42CA5ADE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A418382-8400-4B58-B0C9-C1DD99711D9C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F31C2F9-EC9E-4EF8-B2B9-8ED9767901F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -86,10 +86,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -365,11 +361,11 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1">
-        <f>D1+4</f>
+        <f t="shared" ref="A1:A9" si="0">D1+4</f>
         <v>9</v>
       </c>
       <c r="B1">
-        <f>D1+2</f>
+        <f t="shared" ref="B1:B9" si="1">D1+2</f>
         <v>7</v>
       </c>
       <c r="C1">
@@ -381,11 +377,11 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f>D2+4</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B2">
-        <f>D2+2</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C2">
@@ -397,11 +393,11 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>D3+4</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B3">
-        <f>D3+2</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C3">
@@ -413,11 +409,11 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f>D4+4</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B4">
-        <f>D4+2</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C4">
@@ -429,11 +425,11 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f>D5+4</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B5">
-        <f>D5+2</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C5">
@@ -445,11 +441,11 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f>D6+4</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B6">
-        <f>D6+2</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C6">
@@ -461,11 +457,11 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f>D7+4</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B7">
-        <f>D7+2</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C7">
@@ -477,11 +473,11 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f>D8+4</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8">
-        <f>D8+2</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C8">
@@ -493,11 +489,11 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f>D9+4</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B9">
-        <f>D9+2</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C9">
@@ -516,154 +512,136 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852D3931-4FC5-4B24-A76E-3D4830B987BB}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1">
-        <f>D1-8</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B1">
-        <f>D1-4</f>
         <v>16</v>
       </c>
       <c r="C1">
         <v>16</v>
       </c>
       <c r="D1">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f>D2-8</f>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B2">
-        <f>D2-4</f>
         <v>14</v>
       </c>
       <c r="C2">
         <v>14</v>
       </c>
       <c r="D2">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>D3-8</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B3">
-        <f>D3-4</f>
         <v>12</v>
       </c>
       <c r="C3">
         <v>12</v>
       </c>
       <c r="D3">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f>D4-8</f>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B4">
-        <f>D4-4</f>
         <v>14</v>
       </c>
       <c r="C4">
         <v>14</v>
       </c>
       <c r="D4">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f>D5-8</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B5">
-        <f>D5-4</f>
         <v>12</v>
       </c>
       <c r="C5">
         <v>12</v>
       </c>
       <c r="D5">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f>D6-8</f>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B6">
-        <f>D6-4</f>
         <v>10</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
       <c r="D6">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f>D7-8</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B7">
-        <f>D7-4</f>
         <v>12</v>
       </c>
       <c r="C7">
         <v>12</v>
       </c>
       <c r="D7">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f>D8-8</f>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B8">
-        <f>D8-4</f>
         <v>10</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
       <c r="D8">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f>D9-8</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B9">
-        <f>D9-4</f>
         <v>8</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -693,13 +671,13 @@
         <v>0.7</v>
       </c>
       <c r="D1">
-        <f>B1+0.025</f>
+        <f t="shared" ref="D1:D9" si="0">B1+0.025</f>
         <v>0.72499999999999998</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f t="shared" ref="A2:A9" si="0">B2-0.025</f>
+        <f t="shared" ref="A2:A9" si="1">B2-0.025</f>
         <v>0.72499999999999998</v>
       </c>
       <c r="B2">
@@ -709,13 +687,13 @@
         <v>0.75</v>
       </c>
       <c r="D2">
-        <f>B2+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.77500000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.77500000000000002</v>
       </c>
       <c r="B3">
@@ -725,13 +703,13 @@
         <v>0.8</v>
       </c>
       <c r="D3">
-        <f>B3+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.82500000000000007</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.72499999999999998</v>
       </c>
       <c r="B4">
@@ -741,13 +719,13 @@
         <v>0.75</v>
       </c>
       <c r="D4">
-        <f>B4+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.77500000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.77500000000000002</v>
       </c>
       <c r="B5">
@@ -757,13 +735,13 @@
         <v>0.8</v>
       </c>
       <c r="D5">
-        <f>B5+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.82500000000000007</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.82499999999999996</v>
       </c>
       <c r="B6">
@@ -773,13 +751,13 @@
         <v>0.85</v>
       </c>
       <c r="D6">
-        <f>B6+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.875</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.77500000000000002</v>
       </c>
       <c r="B7">
@@ -789,13 +767,13 @@
         <v>0.8</v>
       </c>
       <c r="D7">
-        <f>B7+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.82500000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.82499999999999996</v>
       </c>
       <c r="B8">
@@ -805,13 +783,13 @@
         <v>0.85</v>
       </c>
       <c r="D8">
-        <f>B8+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.875</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.875</v>
       </c>
       <c r="B9">
@@ -821,7 +799,7 @@
         <v>0.9</v>
       </c>
       <c r="D9">
-        <f>B9+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.92500000000000004</v>
       </c>
     </row>
@@ -834,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E001DE59-3A9C-446C-92E5-5D136716FEDE}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -852,13 +830,13 @@
         <v>0.6</v>
       </c>
       <c r="D1">
-        <f>B1+0.025</f>
+        <f t="shared" ref="D1:D9" si="0">B1+0.025</f>
         <v>0.625</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f t="shared" ref="A2:A9" si="0">B2-0.025</f>
+        <f t="shared" ref="A2:A9" si="1">B2-0.025</f>
         <v>0.625</v>
       </c>
       <c r="B2">
@@ -868,13 +846,13 @@
         <v>0.65</v>
       </c>
       <c r="D2">
-        <f>B2+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.67500000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.67499999999999993</v>
       </c>
       <c r="B3">
@@ -884,13 +862,13 @@
         <v>0.7</v>
       </c>
       <c r="D3">
-        <f>B3+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.72499999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.625</v>
       </c>
       <c r="B4">
@@ -900,13 +878,13 @@
         <v>0.65</v>
       </c>
       <c r="D4">
-        <f>B4+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.67500000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.67499999999999993</v>
       </c>
       <c r="B5">
@@ -916,13 +894,13 @@
         <v>0.7</v>
       </c>
       <c r="D5">
-        <f>B5+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.72499999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.72499999999999998</v>
       </c>
       <c r="B6">
@@ -932,13 +910,13 @@
         <v>0.75</v>
       </c>
       <c r="D6">
-        <f>B6+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.77500000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.67499999999999993</v>
       </c>
       <c r="B7">
@@ -948,13 +926,13 @@
         <v>0.7</v>
       </c>
       <c r="D7">
-        <f>B7+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.72499999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.72499999999999998</v>
       </c>
       <c r="B8">
@@ -964,13 +942,13 @@
         <v>0.75</v>
       </c>
       <c r="D8">
-        <f>B8+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.77500000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.77500000000000002</v>
       </c>
       <c r="B9">
@@ -980,7 +958,7 @@
         <v>0.8</v>
       </c>
       <c r="D9">
-        <f>B9+0.025</f>
+        <f t="shared" si="0"/>
         <v>0.82500000000000007</v>
       </c>
     </row>

</xml_diff>